<commit_message>
add after sales customers process and refactore some part of code.
</commit_message>
<xml_diff>
--- a/components/WEIGHT.xlsx
+++ b/components/WEIGHT.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Havayar\Havayar\Development phase\customer_segmentation\components\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8EDBEAF-2399-4D4E-B04B-D263CFF9550C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D6C85E9-F5B4-47B9-B9DE-ADE91FC3A746}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2790" yWindow="2745" windowWidth="15375" windowHeight="7785" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="routine" sheetId="1" r:id="rId1"/>
     <sheet name="non-routine" sheetId="2" r:id="rId2"/>
-    <sheet name="خدمات هوای فشرده" sheetId="3" r:id="rId3"/>
+    <sheet name="after-sales" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -481,7 +481,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,16 +502,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>0.41949999999999998</v>
+        <v>0.3</v>
       </c>
       <c r="B2" s="1">
-        <v>0.1055</v>
+        <v>0.3</v>
       </c>
       <c r="C2" s="1">
-        <v>5.5599999999999997E-2</v>
+        <v>0.2</v>
       </c>
       <c r="D2" s="1">
-        <v>0.41949999999999998</v>
+        <v>0.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>